<commit_message>
reroute pcb for 40 line lcd screen
</commit_message>
<xml_diff>
--- a/Hardware/Project BOM.xlsx
+++ b/Hardware/Project BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\MSP-Debugger\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94331084-5BEF-4942-885C-4D2FB81F1088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7733697-C3D1-4FA2-8C37-8D68A21BC011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19215" yWindow="15" windowWidth="19185" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4605" yWindow="450" windowWidth="19185" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -833,7 +833,7 @@
   <dimension ref="A1:K996"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fix hardware issues and route small pcb
</commit_message>
<xml_diff>
--- a/Hardware/Project BOM.xlsx
+++ b/Hardware/Project BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\MSP-Debugger\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7733697-C3D1-4FA2-8C37-8D68A21BC011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F8E0E9-97CE-4427-A83B-5E357DF296AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4605" yWindow="450" windowWidth="19185" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17535" yWindow="0" windowWidth="20865" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
   <si>
     <t>Partner 1 Name: Jaden Baptista</t>
   </si>
@@ -323,6 +323,54 @@
   </si>
   <si>
     <t>U4</t>
+  </si>
+  <si>
+    <t>TSW-102-07-G-T</t>
+  </si>
+  <si>
+    <t>TSW-102-07-G-T-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TSW-102-07-G-T/7862063</t>
+  </si>
+  <si>
+    <t>J4, J5</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 6POS 2.54MM</t>
+  </si>
+  <si>
+    <t>https://mm.digikey.com/Volume0/opasdata/d220001/medias/docus/6129/tsw-xxx-xx-xxx-x-xx-xxx-mkt.pdf</t>
+  </si>
+  <si>
+    <t>QPC02SXGN-RC</t>
+  </si>
+  <si>
+    <t>S9337-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/sullins-connector-solutions/QPC02SXGN-RC/2618262</t>
+  </si>
+  <si>
+    <t>CONN JUMPER SHORTING .100" GOLD</t>
+  </si>
+  <si>
+    <t>https://s3.amazonaws.com/catalogspreads-pdf/PAGE128-129%20.100%20JUMPER.pdf</t>
+  </si>
+  <si>
+    <t>AO4882</t>
+  </si>
+  <si>
+    <t>785-1317-1-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/alpha-omega-semiconductor-inc/AO4882/3060989</t>
+  </si>
+  <si>
+    <t>Mosfet Array 40V 8A 2W Surface Mount 8-SOIC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/htmldatasheets/production/1034359/0/0/1/ao4882.pdf</t>
   </si>
 </sst>
 </file>
@@ -830,16 +878,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K996"/>
+  <dimension ref="A1:K998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
     <col min="3" max="3" width="32.42578125" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" customWidth="1"/>
@@ -899,8 +947,8 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="7">
-        <f>SUM(K5:K996)</f>
-        <v>43.593330000000002</v>
+        <f>SUM(K5:K998)</f>
+        <v>46.913330000000002</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1078,11 +1126,11 @@
         <v>1</v>
       </c>
       <c r="J8" s="14">
-        <f t="shared" ref="J8:J28" si="1">A8*I8</f>
+        <f t="shared" ref="J8:J30" si="1">A8*I8</f>
         <v>5</v>
       </c>
       <c r="K8" s="15">
-        <f t="shared" ref="K8:K258" si="2">J8*D8</f>
+        <f t="shared" ref="K8:K260" si="2">J8*D8</f>
         <v>1.1500000000000001</v>
       </c>
     </row>
@@ -1452,83 +1500,133 @@
         <v>1</v>
       </c>
       <c r="K18" s="7">
-        <f t="shared" ref="K18" si="3">J18*D18</f>
+        <f t="shared" ref="K18:K20" si="3">J18*D18</f>
         <v>2.2599999999999998</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="28"/>
+      <c r="A19" s="11">
+        <v>3</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="27">
+        <v>0.52</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="I19" s="28">
+        <v>1</v>
+      </c>
       <c r="J19" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="K19" s="7">
+        <f t="shared" si="3"/>
+        <v>1.56</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="28"/>
+      <c r="A20" s="11">
+        <v>2</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="27">
+        <v>0.73</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="H20" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="I20" s="28">
+        <v>1</v>
+      </c>
       <c r="J20" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="28">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="K20" s="7">
+        <f t="shared" si="3"/>
+        <v>1.46</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="29"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
-      <c r="E21" s="29"/>
+      <c r="A21" s="11">
+        <v>3</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="29" t="s">
+        <v>108</v>
+      </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="28"/>
+      <c r="G21" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="H21" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="I21" s="28">
+        <v>1</v>
+      </c>
       <c r="J21" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K21" s="28">
-        <f>J21*D21</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="29"/>
       <c r="B22" s="29"/>
       <c r="C22" s="29"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="31"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
       <c r="F22" s="29"/>
       <c r="G22" s="29"/>
       <c r="H22" s="29"/>
       <c r="I22" s="28"/>
       <c r="J22" s="14">
-        <f>A22*I22</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K22" s="28">
-        <f>J22*D22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -1536,8 +1634,8 @@
       <c r="A23" s="29"/>
       <c r="B23" s="29"/>
       <c r="C23" s="29"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="31"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
       <c r="F23" s="29"/>
       <c r="G23" s="29"/>
       <c r="H23" s="29"/>
@@ -1555,18 +1653,18 @@
       <c r="A24" s="29"/>
       <c r="B24" s="29"/>
       <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="31"/>
       <c r="F24" s="29"/>
       <c r="G24" s="29"/>
       <c r="H24" s="29"/>
       <c r="I24" s="28"/>
       <c r="J24" s="14">
-        <f t="shared" si="1"/>
+        <f>A24*I24</f>
         <v>0</v>
       </c>
       <c r="K24" s="28">
-        <f t="shared" si="2"/>
+        <f>J24*D24</f>
         <v>0</v>
       </c>
     </row>
@@ -1574,8 +1672,8 @@
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="31"/>
       <c r="F25" s="29"/>
       <c r="G25" s="29"/>
       <c r="H25" s="29"/>
@@ -1585,7 +1683,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="28">
-        <f t="shared" si="2"/>
+        <f>J25*D25</f>
         <v>0</v>
       </c>
     </row>
@@ -1593,8 +1691,8 @@
       <c r="A26" s="29"/>
       <c r="B26" s="29"/>
       <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="31"/>
       <c r="F26" s="29"/>
       <c r="G26" s="29"/>
       <c r="H26" s="29"/>
@@ -1612,8 +1710,8 @@
       <c r="A27" s="29"/>
       <c r="B27" s="29"/>
       <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
+      <c r="D27" s="27"/>
+      <c r="E27" s="31"/>
       <c r="F27" s="29"/>
       <c r="G27" s="29"/>
       <c r="H27" s="29"/>
@@ -1631,8 +1729,8 @@
       <c r="A28" s="29"/>
       <c r="B28" s="29"/>
       <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
+      <c r="D28" s="27"/>
+      <c r="E28" s="31"/>
       <c r="F28" s="29"/>
       <c r="G28" s="29"/>
       <c r="H28" s="29"/>
@@ -1650,14 +1748,14 @@
       <c r="A29" s="29"/>
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
+      <c r="D29" s="27"/>
       <c r="E29" s="29"/>
       <c r="F29" s="29"/>
       <c r="G29" s="29"/>
       <c r="H29" s="29"/>
       <c r="I29" s="28"/>
-      <c r="J29" s="28">
-        <f t="shared" ref="J29:J258" si="4">A29*I29</f>
+      <c r="J29" s="14">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K29" s="28">
@@ -1669,14 +1767,14 @@
       <c r="A30" s="29"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
+      <c r="D30" s="27"/>
       <c r="E30" s="29"/>
       <c r="F30" s="29"/>
       <c r="G30" s="29"/>
       <c r="H30" s="29"/>
       <c r="I30" s="28"/>
-      <c r="J30" s="28">
-        <f t="shared" si="4"/>
+      <c r="J30" s="14">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K30" s="28">
@@ -1688,14 +1786,14 @@
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
+      <c r="D31" s="27"/>
       <c r="E31" s="29"/>
       <c r="F31" s="29"/>
       <c r="G31" s="29"/>
       <c r="H31" s="29"/>
       <c r="I31" s="28"/>
       <c r="J31" s="28">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="J31:J260" si="4">A31*I31</f>
         <v>0</v>
       </c>
       <c r="K31" s="28">
@@ -1707,7 +1805,7 @@
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
+      <c r="D32" s="27"/>
       <c r="E32" s="29"/>
       <c r="F32" s="29"/>
       <c r="G32" s="29"/>
@@ -1726,7 +1824,7 @@
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
+      <c r="D33" s="27"/>
       <c r="E33" s="29"/>
       <c r="F33" s="29"/>
       <c r="G33" s="29"/>
@@ -6027,11 +6125,11 @@
       <c r="H259" s="29"/>
       <c r="I259" s="28"/>
       <c r="J259" s="28">
-        <f t="shared" ref="J259:J513" si="5">A259*I259</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K259" s="28">
-        <f t="shared" ref="K259:K513" si="6">J259*D259</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6046,11 +6144,11 @@
       <c r="H260" s="29"/>
       <c r="I260" s="28"/>
       <c r="J260" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K260" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -6065,11 +6163,11 @@
       <c r="H261" s="29"/>
       <c r="I261" s="28"/>
       <c r="J261" s="28">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="J261:J515" si="5">A261*I261</f>
         <v>0</v>
       </c>
       <c r="K261" s="28">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="K261:K515" si="6">J261*D261</f>
         <v>0</v>
       </c>
     </row>
@@ -10872,11 +10970,11 @@
       <c r="H514" s="29"/>
       <c r="I514" s="28"/>
       <c r="J514" s="28">
-        <f t="shared" ref="J514:J768" si="7">A514*I514</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K514" s="28">
-        <f t="shared" ref="K514:K768" si="8">J514*D514</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10891,11 +10989,11 @@
       <c r="H515" s="29"/>
       <c r="I515" s="28"/>
       <c r="J515" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="K515" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
@@ -10910,11 +11008,11 @@
       <c r="H516" s="29"/>
       <c r="I516" s="28"/>
       <c r="J516" s="28">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="J516:J770" si="7">A516*I516</f>
         <v>0</v>
       </c>
       <c r="K516" s="28">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="K516:K770" si="8">J516*D516</f>
         <v>0</v>
       </c>
     </row>
@@ -15717,11 +15815,11 @@
       <c r="H769" s="29"/>
       <c r="I769" s="28"/>
       <c r="J769" s="28">
-        <f t="shared" ref="J769:J996" si="9">A769*I769</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K769" s="28">
-        <f t="shared" ref="K769:K996" si="10">J769*D769</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -15736,11 +15834,11 @@
       <c r="H770" s="29"/>
       <c r="I770" s="28"/>
       <c r="J770" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K770" s="28">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
     </row>
@@ -15755,11 +15853,11 @@
       <c r="H771" s="29"/>
       <c r="I771" s="28"/>
       <c r="J771" s="28">
-        <f t="shared" si="9"/>
+        <f t="shared" ref="J771:J998" si="9">A771*I771</f>
         <v>0</v>
       </c>
       <c r="K771" s="28">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="K771:K998" si="10">J771*D771</f>
         <v>0</v>
       </c>
     </row>
@@ -20034,6 +20132,44 @@
         <v>0</v>
       </c>
       <c r="K996" s="28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="997" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A997" s="29"/>
+      <c r="B997" s="29"/>
+      <c r="C997" s="29"/>
+      <c r="D997" s="29"/>
+      <c r="E997" s="29"/>
+      <c r="F997" s="29"/>
+      <c r="G997" s="29"/>
+      <c r="H997" s="29"/>
+      <c r="I997" s="28"/>
+      <c r="J997" s="28">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K997" s="28">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="998" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A998" s="29"/>
+      <c r="B998" s="29"/>
+      <c r="C998" s="29"/>
+      <c r="D998" s="29"/>
+      <c r="E998" s="29"/>
+      <c r="F998" s="29"/>
+      <c r="G998" s="29"/>
+      <c r="H998" s="29"/>
+      <c r="I998" s="28"/>
+      <c r="J998" s="28">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="K998" s="28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
gerber pcb and update BOM
</commit_message>
<xml_diff>
--- a/Hardware/Project BOM.xlsx
+++ b/Hardware/Project BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\MSP-Debugger\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F8E0E9-97CE-4427-A83B-5E357DF296AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D070384-36B9-48E0-A2E4-B1D847214965}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17535" yWindow="0" windowWidth="20865" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="125">
   <si>
     <t>Partner 1 Name: Jaden Baptista</t>
   </si>
@@ -371,6 +371,33 @@
   </si>
   <si>
     <t>https://www.digikey.com/htmldatasheets/production/1034359/0/0/1/ao4882.pdf</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 18POS 2.54MM</t>
+  </si>
+  <si>
+    <t>TD-109-T-A</t>
+  </si>
+  <si>
+    <t>SAM1114-09-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TD-109-T-A/1105549</t>
+  </si>
+  <si>
+    <t>https://suddendocs.samtec.com/catalog_english/td.pdf</t>
+  </si>
+  <si>
+    <t>TS-110-T-A</t>
+  </si>
+  <si>
+    <t>SAM1112-10-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/samtec-inc/TS-110-T-A/1105484</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 10POS 2.54MM</t>
   </si>
 </sst>
 </file>
@@ -881,7 +908,7 @@
   <dimension ref="A1:K998"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -948,7 +975,7 @@
       <c r="J3" s="5"/>
       <c r="K3" s="7">
         <f>SUM(K5:K998)</f>
-        <v>46.913330000000002</v>
+        <v>59.543329999999997</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1025,7 +1052,7 @@
     </row>
     <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B6" s="17" t="s">
         <v>22</v>
@@ -1053,11 +1080,11 @@
       </c>
       <c r="J6" s="14">
         <f>A6*I6</f>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="K6" s="7">
         <f>J6*D6</f>
-        <v>0.2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1099,7 +1126,7 @@
     </row>
     <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="17" t="s">
         <v>17</v>
@@ -1127,11 +1154,11 @@
       </c>
       <c r="J8" s="14">
         <f t="shared" ref="J8:J30" si="1">A8*I8</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K8" s="15">
         <f t="shared" ref="K8:K260" si="2">J8*D8</f>
-        <v>1.1500000000000001</v>
+        <v>1.3800000000000001</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1506,7 +1533,7 @@
     </row>
     <row r="19" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>111</v>
@@ -1532,11 +1559,11 @@
       </c>
       <c r="J19" s="14">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K19" s="7">
         <f t="shared" si="3"/>
-        <v>1.56</v>
+        <v>2.08</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1589,7 +1616,7 @@
       <c r="D21" s="27">
         <v>0.1</v>
       </c>
-      <c r="E21" s="29" t="s">
+      <c r="E21" s="31" t="s">
         <v>108</v>
       </c>
       <c r="F21" s="29"/>
@@ -1612,41 +1639,73 @@
       </c>
     </row>
     <row r="22" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
+      <c r="A22" s="29">
+        <v>2</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="27">
+        <v>3.6</v>
+      </c>
+      <c r="E22" s="31" t="s">
+        <v>119</v>
+      </c>
       <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="28"/>
+      <c r="G22" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="H22" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="I22" s="28">
+        <v>1</v>
+      </c>
       <c r="J22" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K22" s="28">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
+      <c r="A23" s="29">
+        <v>2</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1.94</v>
+      </c>
+      <c r="E23" s="31" t="s">
+        <v>123</v>
+      </c>
       <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="28"/>
+      <c r="G23" s="29" t="s">
+        <v>124</v>
+      </c>
+      <c r="H23" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="I23" s="28">
+        <v>1</v>
+      </c>
       <c r="J23" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K23" s="28">
         <f>J23*D23</f>
-        <v>0</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -20204,6 +20263,11 @@
     <hyperlink ref="E7" r:id="rId23" xr:uid="{1631215A-648B-47D2-9E16-3378AF6A2FCA}"/>
     <hyperlink ref="E6" r:id="rId24" xr:uid="{F9C48F87-B949-497A-BEF6-E2E32E12AC07}"/>
     <hyperlink ref="H6" r:id="rId25" xr:uid="{92CFB618-DB03-47DC-8056-C042921B1798}"/>
+    <hyperlink ref="E20" r:id="rId26" xr:uid="{E4E10181-3531-49A2-BDDB-D58398CB3A73}"/>
+    <hyperlink ref="E19" r:id="rId27" xr:uid="{4162E094-2CCA-4900-A73C-FB61512403D4}"/>
+    <hyperlink ref="E21" r:id="rId28" xr:uid="{08F6B92E-E585-45F0-8B4E-DE3B0BEE0AAD}"/>
+    <hyperlink ref="E22" r:id="rId29" xr:uid="{FCD33A3C-B975-424E-9F39-F669205479DE}"/>
+    <hyperlink ref="E23" r:id="rId30" xr:uid="{8EE4FA0F-5C45-4F23-A5AD-19AC8B0FAE2B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>